<commit_message>
feat: update `MAX_PD_XXX_SIZE` in esp
</commit_message>
<xml_diff>
--- a/Core/Src/SSC/SSC-Device.xlsx
+++ b/Core/Src/SSC/SSC-Device.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\bensung\expm_SSC\Core\Src\SSC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87671A6F-B012-4886-B8D4-1933279534E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22267198-5CD5-4BA4-8B0B-1A49E4D930C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -891,8 +891,8 @@
   <dimension ref="A1:T67"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="10" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G38" sqref="G38"/>
+      <pane ySplit="10" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M43" sqref="M43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
feat: runtime PDO mapping implementation
</commit_message>
<xml_diff>
--- a/Core/Src/SSC/SSC-Device.xlsx
+++ b/Core/Src/SSC/SSC-Device.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\bensung\expm_SSC\Core\Src\SSC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22267198-5CD5-4BA4-8B0B-1A49E4D930C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4634AC2-A37C-4597-B8B2-A5169F47F1BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="78">
   <si>
     <t>Device Profile:</t>
   </si>
@@ -378,6 +378,10 @@
   </si>
   <si>
     <t>Change polarity output 01h to 08h</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>rx</t>
     <phoneticPr fontId="7" type="noConversion"/>
   </si>
 </sst>
@@ -891,8 +895,8 @@
   <dimension ref="A1:T67"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="10" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M43" sqref="M43"/>
+      <pane ySplit="10" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -920,7 +924,7 @@
         <v>0</v>
       </c>
       <c r="C1" s="2">
-        <v>5001</v>
+        <v>0</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>1</v>
@@ -1743,6 +1747,9 @@
       <c r="L43" t="s">
         <v>64</v>
       </c>
+      <c r="M43" t="s">
+        <v>77</v>
+      </c>
       <c r="P43" t="s">
         <v>73</v>
       </c>

</xml_diff>